<commit_message>
read WayPoints database as xlsx file
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
+++ b/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\04 - Workspace\flight-profile\airline\management\commands\AirlineRoutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2394EF7-0A5A-446C-AFD1-191677942CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8785C9-27BA-44C4-882D-DB8C41FC7783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="3765" windowWidth="26490" windowHeight="12630"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>Departure Airport</t>
   </si>
@@ -156,12 +156,24 @@
   </si>
   <si>
     <t>Los Angeles Intl</t>
+  </si>
+  <si>
+    <t>LFOB</t>
+  </si>
+  <si>
+    <t>Paris-Beauvais-Tille</t>
+  </si>
+  <si>
+    <t>Hungary-Budapest-Listz</t>
+  </si>
+  <si>
+    <t>LHBP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,11 +521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,6 +860,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
retrieve an xlsx file with the computed profile
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
+++ b/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\04 - Workspace\flight-profile\airline\management\commands\AirlineRoutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8785C9-27BA-44C4-882D-DB8C41FC7783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B705F8-EAEC-47BB-A7C8-2BC25A5F881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1875" yWindow="2970" windowWidth="26490" windowHeight="12630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
   <si>
     <t>Departure Airport</t>
   </si>
@@ -522,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D21" sqref="D21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,6 +877,23 @@
         <v>44</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add new indian routes
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
+++ b/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\04 - Workspace\flight-profile\airline\management\commands\AirlineRoutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B705F8-EAEC-47BB-A7C8-2BC25A5F881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7CCA08-BF90-49AF-ACE1-52A4A3C51E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="2970" windowWidth="26490" windowHeight="12630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1755" yWindow="1410" windowWidth="26490" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
   <si>
     <t>Departure Airport</t>
   </si>
@@ -168,6 +168,30 @@
   </si>
   <si>
     <t>LHBP</t>
+  </si>
+  <si>
+    <t>VABB</t>
+  </si>
+  <si>
+    <t>Mumbai-India</t>
+  </si>
+  <si>
+    <t>VECC</t>
+  </si>
+  <si>
+    <t>Calcutta-India</t>
+  </si>
+  <si>
+    <t>Chennai-India</t>
+  </si>
+  <si>
+    <t>VOMM</t>
+  </si>
+  <si>
+    <t>Jaipur-India</t>
+  </si>
+  <si>
+    <t>VIJP</t>
   </si>
 </sst>
 </file>
@@ -522,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:E21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,53 +869,87 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>41</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add route from Mexico to Seatle
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
+++ b/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\04 - Workspace\flight-profile\airline\management\commands\AirlineRoutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\git\flight-profile\airline\management\commands\AirlineRoutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7CCA08-BF90-49AF-ACE1-52A4A3C51E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8344E765-354C-424D-97DA-43140536C2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="1410" windowWidth="26490" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>Departure Airport</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>VIJP</t>
+  </si>
+  <si>
+    <t>MMMX</t>
+  </si>
+  <si>
+    <t>Aeropuerto México Ciudad Intl</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -549,19 +555,19 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -578,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -595,7 +601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -612,24 +618,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -646,7 +652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -663,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -680,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -697,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -714,7 +720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -731,7 +737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -748,7 +754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -765,7 +771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -782,7 +788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -799,7 +805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -816,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -833,7 +839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -850,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -867,7 +873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -884,7 +890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -901,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -918,7 +924,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -935,7 +941,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
add new route from Madrid Barajas to Berlin Brandebourg
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
+++ b/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\git\flight-profile\airline\management\commands\AirlineRoutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8344E765-354C-424D-97DA-43140536C2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF2BE2D-C5B0-49A8-9DFA-77C4F9B860D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
   <si>
     <t>Departure Airport</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t>Aeropuerto México Ciudad Intl</t>
+  </si>
+  <si>
+    <t>Madrid-Barajas</t>
+  </si>
+  <si>
+    <t>Berlin-Brandenburg</t>
+  </si>
+  <si>
+    <t>EDDB</t>
+  </si>
+  <si>
+    <t>LEMD</t>
   </si>
 </sst>
 </file>
@@ -552,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -909,19 +921,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -929,16 +941,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -946,15 +958,32 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
extend european routes with Faro to Brussels
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
+++ b/airline/management/commands/AirlineRoutes/AirlineRoutesAirportsDepartureArrival.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\git\flight-profile\airline\management\commands\AirlineRoutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF2BE2D-C5B0-49A8-9DFA-77C4F9B860D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6268EB03-FF52-4376-A9AA-1880EBEF47F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>Departure Airport</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>LEMD</t>
+  </si>
+  <si>
+    <t>EBBR</t>
+  </si>
+  <si>
+    <t>Faro-Portugal</t>
+  </si>
+  <si>
+    <t>Brussels-National</t>
+  </si>
+  <si>
+    <t>LPFR</t>
   </si>
 </sst>
 </file>
@@ -268,9 +280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -414,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,19 +950,19 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -958,16 +970,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -975,15 +987,32 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>